<commit_message>
user registration form and routes!
</commit_message>
<xml_diff>
--- a/Component Architecture Basic.xlsx
+++ b/Component Architecture Basic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Training\CTS\Feb 2020 HTML5 CSS3 Typescript Angular - Deepti\Examples\angularapp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20B69CAA-3E2A-4953-86CA-6F835E103585}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{179E1E01-5BC4-476D-8691-2682E99A4691}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31515" yWindow="660" windowWidth="21600" windowHeight="14895" xr2:uid="{9CD3BF59-CF7B-4014-BF9C-531509676BB2}"/>
+    <workbookView xWindow="29655" yWindow="660" windowWidth="27795" windowHeight="14895" xr2:uid="{9CD3BF59-CF7B-4014-BF9C-531509676BB2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
   <si>
     <t>Root Module</t>
   </si>
@@ -137,9 +137,6 @@
     <t>carousel</t>
   </si>
   <si>
-    <t>user registration component</t>
-  </si>
-  <si>
     <t>template/reactive form</t>
   </si>
   <si>
@@ -153,6 +150,39 @@
   </si>
   <si>
     <t>free stock images -&gt; https://www.freeimages.com/</t>
+  </si>
+  <si>
+    <t>Registration form on slideshow</t>
+  </si>
+  <si>
+    <t>registration component</t>
+  </si>
+  <si>
+    <t>user registration component (child of slideshow component)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implementing routes </t>
+  </si>
+  <si>
+    <t>All possible routes without authenticatio and authorization!</t>
+  </si>
+  <si>
+    <t>Home</t>
+  </si>
+  <si>
+    <t>All Shops</t>
+  </si>
+  <si>
+    <t>Add New Shop</t>
+  </si>
+  <si>
+    <t>Shop Detail</t>
+  </si>
+  <si>
+    <t>About Us</t>
+  </si>
+  <si>
+    <t>Contact Us</t>
   </si>
 </sst>
 </file>
@@ -507,16 +537,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C80F6326-BE78-4A18-8AE8-A2A418690DC0}">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42:D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="74.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="47.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.42578125" bestFit="1" customWidth="1"/>
@@ -602,10 +632,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" t="s">
         <v>34</v>
-      </c>
-      <c r="F11" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -690,18 +720,68 @@
         <v>2</v>
       </c>
       <c r="B33" t="s">
+        <v>35</v>
+      </c>
+      <c r="C33" t="s">
         <v>36</v>
-      </c>
-      <c r="C33" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
+        <v>37</v>
+      </c>
+      <c r="D34" t="s">
         <v>38</v>
       </c>
-      <c r="D34" t="s">
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>3</v>
+      </c>
+      <c r="B35" t="s">
         <v>39</v>
+      </c>
+      <c r="C35" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>4</v>
+      </c>
+      <c r="B36" t="s">
+        <v>42</v>
+      </c>
+      <c r="C36" t="s">
+        <v>43</v>
+      </c>
+      <c r="D36" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D39" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
user registration and add new shop
</commit_message>
<xml_diff>
--- a/Component Architecture Basic.xlsx
+++ b/Component Architecture Basic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Training\CTS\Feb 2020 HTML5 CSS3 Typescript Angular - Deepti\Examples\angularapp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{179E1E01-5BC4-476D-8691-2682E99A4691}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED81E4D-AA3B-430C-A66B-2D40A9A86F11}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29655" yWindow="660" windowWidth="27795" windowHeight="14895" xr2:uid="{9CD3BF59-CF7B-4014-BF9C-531509676BB2}"/>
+    <workbookView xWindow="35595" yWindow="615" windowWidth="20370" windowHeight="13035" xr2:uid="{9CD3BF59-CF7B-4014-BF9C-531509676BB2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="57">
   <si>
     <t>Root Module</t>
   </si>
@@ -164,9 +164,6 @@
     <t xml:space="preserve">Implementing routes </t>
   </si>
   <si>
-    <t>All possible routes without authenticatio and authorization!</t>
-  </si>
-  <si>
     <t>Home</t>
   </si>
   <si>
@@ -183,6 +180,30 @@
   </si>
   <si>
     <t>Contact Us</t>
+  </si>
+  <si>
+    <t>All possible routes without authentication and authorization!</t>
+  </si>
+  <si>
+    <t>Tempalte Driven Form</t>
+  </si>
+  <si>
+    <t>User Registration on Home Page</t>
+  </si>
+  <si>
+    <t>Service for using all REST endpoints</t>
+  </si>
+  <si>
+    <t>json-server</t>
+  </si>
+  <si>
+    <t>Create Fake REST end points</t>
+  </si>
+  <si>
+    <t>Add New Shop Template Driven Form</t>
+  </si>
+  <si>
+    <t>Service for add new shop</t>
   </si>
 </sst>
 </file>
@@ -537,10 +558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C80F6326-BE78-4A18-8AE8-A2A418690DC0}">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42:D43"/>
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -753,35 +774,69 @@
         <v>42</v>
       </c>
       <c r="C36" t="s">
+        <v>49</v>
+      </c>
+      <c r="D36" t="s">
         <v>43</v>
-      </c>
-      <c r="D36" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D37" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D38" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D41" t="s">
-        <v>49</v>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>5</v>
+      </c>
+      <c r="B42" t="s">
+        <v>50</v>
+      </c>
+      <c r="C42" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>54</v>
+      </c>
+      <c r="D44" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>